<commit_message>
2019-10-15 20:24 tablas corregidas
</commit_message>
<xml_diff>
--- a/resultados/pretratamiento-tablas-control/pretrat-alemania-elo-dificil-dificultad.xlsx
+++ b/resultados/pretratamiento-tablas-control/pretrat-alemania-elo-dificil-dificultad.xlsx
@@ -3572,10 +3572,10 @@
         <v>-1.515</v>
       </c>
       <c r="H2">
-        <v>-0.389</v>
+        <v>-0.351</v>
       </c>
       <c r="I2">
-        <v>0.698</v>
+        <v>0.725</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3601,10 +3601,10 @@
         <v>4.116</v>
       </c>
       <c r="H3">
-        <v>1.111</v>
+        <v>1.333</v>
       </c>
       <c r="I3">
-        <v>0.268</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3630,10 +3630,10 @@
         <v>0.365</v>
       </c>
       <c r="H4">
-        <v>0.08599999999999999</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="I4">
-        <v>0.931</v>
+        <v>0.945</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3659,10 +3659,10 @@
         <v>1.527</v>
       </c>
       <c r="H5">
-        <v>0.376</v>
+        <v>0.338</v>
       </c>
       <c r="I5">
-        <v>0.707</v>
+        <v>0.736</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3688,10 +3688,10 @@
         <v>-4.65</v>
       </c>
       <c r="H6">
-        <v>-1.096</v>
+        <v>-0.828</v>
       </c>
       <c r="I6">
-        <v>0.274</v>
+        <v>0.408</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3717,10 +3717,10 @@
         <v>-5.113</v>
       </c>
       <c r="H7">
-        <v>-1.063</v>
+        <v>-1.37</v>
       </c>
       <c r="I7">
-        <v>0.289</v>
+        <v>0.171</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3746,10 +3746,10 @@
         <v>0.657</v>
       </c>
       <c r="H8">
-        <v>0.394</v>
+        <v>0.335</v>
       </c>
       <c r="I8">
-        <v>0.694</v>
+        <v>0.738</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3775,10 +3775,10 @@
         <v>-1.938</v>
       </c>
       <c r="H9">
-        <v>-1.207</v>
+        <v>-1.342</v>
       </c>
       <c r="I9">
-        <v>0.229</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3804,10 +3804,10 @@
         <v>-0.706</v>
       </c>
       <c r="H10">
-        <v>-0.4</v>
+        <v>-0.319</v>
       </c>
       <c r="I10">
-        <v>0.6899999999999999</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3833,10 +3833,10 @@
         <v>-0.09</v>
       </c>
       <c r="H11">
-        <v>-0.051</v>
+        <v>-0.043</v>
       </c>
       <c r="I11">
-        <v>0.96</v>
+        <v>0.965</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3862,10 +3862,10 @@
         <v>2.059</v>
       </c>
       <c r="H12">
-        <v>1.165</v>
+        <v>0.913</v>
       </c>
       <c r="I12">
-        <v>0.245</v>
+        <v>0.361</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3891,10 +3891,10 @@
         <v>1.598</v>
       </c>
       <c r="H13">
-        <v>0.901</v>
+        <v>1.079</v>
       </c>
       <c r="I13">
-        <v>0.369</v>
+        <v>0.281</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3920,10 +3920,10 @@
         <v>0.003</v>
       </c>
       <c r="H14">
-        <v>0.136</v>
+        <v>0.13</v>
       </c>
       <c r="I14">
-        <v>0.892</v>
+        <v>0.897</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3949,10 +3949,10 @@
         <v>0.036</v>
       </c>
       <c r="H15">
-        <v>1.474</v>
+        <v>1.294</v>
       </c>
       <c r="I15">
-        <v>0.142</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3978,10 +3978,10 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="H16">
-        <v>0.35</v>
+        <v>0.234</v>
       </c>
       <c r="I16">
-        <v>0.726</v>
+        <v>0.8149999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -4007,10 +4007,10 @@
         <v>-0.04</v>
       </c>
       <c r="H17">
-        <v>-1.463</v>
+        <v>-1.299</v>
       </c>
       <c r="I17">
-        <v>0.145</v>
+        <v>0.194</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -4036,10 +4036,10 @@
         <v>-0.014</v>
       </c>
       <c r="H18">
-        <v>-0.441</v>
+        <v>-0.403</v>
       </c>
       <c r="I18">
-        <v>0.659</v>
+        <v>0.6870000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -4065,10 +4065,10 @@
         <v>0.037</v>
       </c>
       <c r="H19">
-        <v>1.086</v>
+        <v>1.276</v>
       </c>
       <c r="I19">
-        <v>0.279</v>
+        <v>0.202</v>
       </c>
     </row>
   </sheetData>
@@ -4154,10 +4154,10 @@
         <v>3.678</v>
       </c>
       <c r="I2">
-        <v>0.724</v>
+        <v>0.535</v>
       </c>
       <c r="J2">
-        <v>0.47</v>
+        <v>0.593</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4186,10 +4186,10 @@
         <v>7.61</v>
       </c>
       <c r="I3">
-        <v>1.642</v>
+        <v>1.272</v>
       </c>
       <c r="J3">
-        <v>0.103</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4218,10 +4218,10 @@
         <v>9.821999999999999</v>
       </c>
       <c r="I4">
-        <v>1.792</v>
+        <v>1.513</v>
       </c>
       <c r="J4">
-        <v>0.075</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -4250,10 +4250,10 @@
         <v>-4.982</v>
       </c>
       <c r="I5">
-        <v>-0.954</v>
+        <v>-0.853</v>
       </c>
       <c r="J5">
-        <v>0.342</v>
+        <v>0.394</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4282,10 +4282,10 @@
         <v>-3.919</v>
       </c>
       <c r="I6">
-        <v>-0.726</v>
+        <v>-0.593</v>
       </c>
       <c r="J6">
-        <v>0.469</v>
+        <v>0.553</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4314,10 +4314,10 @@
         <v>-3.247</v>
       </c>
       <c r="I7">
-        <v>-0.502</v>
+        <v>-0.522</v>
       </c>
       <c r="J7">
-        <v>0.616</v>
+        <v>0.601</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4346,10 +4346,10 @@
         <v>-1.574</v>
       </c>
       <c r="I8">
-        <v>-0.707</v>
+        <v>-0.594</v>
       </c>
       <c r="J8">
-        <v>0.48</v>
+        <v>0.552</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4378,10 +4378,10 @@
         <v>-4.092</v>
       </c>
       <c r="I9">
-        <v>-1.997</v>
+        <v>-1.601</v>
       </c>
       <c r="J9">
-        <v>0.048</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4410,10 +4410,10 @@
         <v>-4.857</v>
       </c>
       <c r="I10">
-        <v>-2.094</v>
+        <v>-1.709</v>
       </c>
       <c r="J10">
-        <v>0.038</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4442,10 +4442,10 @@
         <v>1.966</v>
       </c>
       <c r="I11">
-        <v>0.837</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="J11">
-        <v>0.404</v>
+        <v>0.495</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -4474,10 +4474,10 @@
         <v>2.042</v>
       </c>
       <c r="I12">
-        <v>0.887</v>
+        <v>0.759</v>
       </c>
       <c r="J12">
-        <v>0.376</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -4506,7 +4506,7 @@
         <v>0.039</v>
       </c>
       <c r="I13">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="J13">
         <v>0.987</v>
@@ -4538,10 +4538,10 @@
         <v>-0.019</v>
       </c>
       <c r="I14">
-        <v>-0.609</v>
+        <v>-0.701</v>
       </c>
       <c r="J14">
-        <v>0.544</v>
+        <v>0.483</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -4570,10 +4570,10 @@
         <v>-0.051</v>
       </c>
       <c r="I15">
-        <v>-1.546</v>
+        <v>-1.159</v>
       </c>
       <c r="J15">
-        <v>0.124</v>
+        <v>0.247</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -4602,10 +4602,10 @@
         <v>-0.018</v>
       </c>
       <c r="I16">
-        <v>-0.511</v>
+        <v>-0.392</v>
       </c>
       <c r="J16">
-        <v>0.61</v>
+        <v>0.695</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -4634,10 +4634,10 @@
         <v>-0.076</v>
       </c>
       <c r="I17">
-        <v>-2.033</v>
+        <v>-1.551</v>
       </c>
       <c r="J17">
-        <v>0.044</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -4666,10 +4666,10 @@
         <v>-0.011</v>
       </c>
       <c r="I18">
-        <v>-0.263</v>
+        <v>-0.296</v>
       </c>
       <c r="J18">
-        <v>0.793</v>
+        <v>0.767</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -4698,10 +4698,10 @@
         <v>0.055</v>
       </c>
       <c r="I19">
-        <v>1.283</v>
+        <v>1.426</v>
       </c>
       <c r="J19">
-        <v>0.202</v>
+        <v>0.154</v>
       </c>
     </row>
   </sheetData>
@@ -4787,10 +4787,10 @@
         <v>5.99</v>
       </c>
       <c r="I2">
-        <v>1.038</v>
+        <v>0.865</v>
       </c>
       <c r="J2">
-        <v>0.301</v>
+        <v>0.387</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4819,10 +4819,10 @@
         <v>3.059</v>
       </c>
       <c r="I3">
-        <v>0.575</v>
+        <v>0.555</v>
       </c>
       <c r="J3">
-        <v>0.5659999999999999</v>
+        <v>0.579</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4851,10 +4851,10 @@
         <v>2.532</v>
       </c>
       <c r="I4">
-        <v>0.402</v>
+        <v>0.398</v>
       </c>
       <c r="J4">
-        <v>0.6889999999999999</v>
+        <v>0.6909999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -4883,10 +4883,10 @@
         <v>-11.522</v>
       </c>
       <c r="I5">
-        <v>-1.957</v>
+        <v>-2.012</v>
       </c>
       <c r="J5">
-        <v>0.052</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4915,10 +4915,10 @@
         <v>-11.318</v>
       </c>
       <c r="I6">
-        <v>-1.861</v>
+        <v>-1.314</v>
       </c>
       <c r="J6">
-        <v>0.065</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4947,10 +4947,10 @@
         <v>-15.599</v>
       </c>
       <c r="I7">
-        <v>-2.15</v>
+        <v>-1.915</v>
       </c>
       <c r="J7">
-        <v>0.033</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4979,10 +4979,10 @@
         <v>-2.53</v>
       </c>
       <c r="I8">
-        <v>-1</v>
+        <v>-0.957</v>
       </c>
       <c r="J8">
-        <v>0.319</v>
+        <v>0.339</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5011,10 +5011,10 @@
         <v>-1.972</v>
       </c>
       <c r="I9">
-        <v>-0.836</v>
+        <v>-0.848</v>
       </c>
       <c r="J9">
-        <v>0.404</v>
+        <v>0.396</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5043,10 +5043,10 @@
         <v>-0.755</v>
       </c>
       <c r="I10">
-        <v>-0.282</v>
+        <v>-0.259</v>
       </c>
       <c r="J10">
-        <v>0.778</v>
+        <v>0.796</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5075,10 +5075,10 @@
         <v>5.088</v>
       </c>
       <c r="I11">
-        <v>1.922</v>
+        <v>1.744</v>
       </c>
       <c r="J11">
-        <v>0.057</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5107,10 +5107,10 @@
         <v>5.097</v>
       </c>
       <c r="I12">
-        <v>1.965</v>
+        <v>1.467</v>
       </c>
       <c r="J12">
-        <v>0.051</v>
+        <v>0.142</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5139,10 +5139,10 @@
         <v>4.105</v>
       </c>
       <c r="I13">
-        <v>1.531</v>
+        <v>1.382</v>
       </c>
       <c r="J13">
-        <v>0.128</v>
+        <v>0.167</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5171,10 +5171,10 @@
         <v>-0.05</v>
       </c>
       <c r="I14">
-        <v>-1.437</v>
+        <v>-1.157</v>
       </c>
       <c r="J14">
-        <v>0.153</v>
+        <v>0.247</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5203,10 +5203,10 @@
         <v>-0.09</v>
       </c>
       <c r="I15">
-        <v>-2.418</v>
+        <v>-1.586</v>
       </c>
       <c r="J15">
-        <v>0.017</v>
+        <v>0.113</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5235,10 +5235,10 @@
         <v>-0.004</v>
       </c>
       <c r="I16">
-        <v>-0.109</v>
+        <v>-0.099</v>
       </c>
       <c r="J16">
-        <v>0.913</v>
+        <v>0.921</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5267,10 +5267,10 @@
         <v>-0.08699999999999999</v>
       </c>
       <c r="I17">
-        <v>-2.045</v>
+        <v>-1.48</v>
       </c>
       <c r="J17">
-        <v>0.043</v>
+        <v>0.139</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5299,10 +5299,10 @@
         <v>-0.012</v>
       </c>
       <c r="I18">
-        <v>-0.261</v>
+        <v>-0.236</v>
       </c>
       <c r="J18">
-        <v>0.794</v>
+        <v>0.8129999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5331,10 +5331,10 @@
         <v>-0.021</v>
       </c>
       <c r="I19">
-        <v>-0.44</v>
+        <v>-0.426</v>
       </c>
       <c r="J19">
-        <v>0.661</v>
+        <v>0.67</v>
       </c>
     </row>
   </sheetData>
@@ -5420,10 +5420,10 @@
         <v>1.502</v>
       </c>
       <c r="I2">
-        <v>0.236</v>
+        <v>0.206</v>
       </c>
       <c r="J2">
-        <v>0.8139999999999999</v>
+        <v>0.837</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5452,10 +5452,10 @@
         <v>2.605</v>
       </c>
       <c r="I3">
-        <v>0.445</v>
+        <v>0.367</v>
       </c>
       <c r="J3">
-        <v>0.657</v>
+        <v>0.714</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5484,10 +5484,10 @@
         <v>-1.417</v>
       </c>
       <c r="I4">
-        <v>-0.204</v>
+        <v>-0.232</v>
       </c>
       <c r="J4">
-        <v>0.838</v>
+        <v>0.8169999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5516,10 +5516,10 @@
         <v>-11.949</v>
       </c>
       <c r="I5">
-        <v>-1.842</v>
+        <v>-1.316</v>
       </c>
       <c r="J5">
-        <v>0.067</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5548,10 +5548,10 @@
         <v>-14.364</v>
       </c>
       <c r="I6">
-        <v>-2.155</v>
+        <v>-1.804</v>
       </c>
       <c r="J6">
-        <v>0.033</v>
+        <v>0.07099999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5580,10 +5580,10 @@
         <v>-10.568</v>
       </c>
       <c r="I7">
-        <v>-1.311</v>
+        <v>-1.221</v>
       </c>
       <c r="J7">
-        <v>0.192</v>
+        <v>0.222</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5612,10 +5612,10 @@
         <v>-0.33</v>
       </c>
       <c r="I8">
-        <v>-0.118</v>
+        <v>-0.115</v>
       </c>
       <c r="J8">
-        <v>0.906</v>
+        <v>0.908</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5644,10 +5644,10 @@
         <v>-1.628</v>
       </c>
       <c r="I9">
-        <v>-0.627</v>
+        <v>-0.617</v>
       </c>
       <c r="J9">
-        <v>0.532</v>
+        <v>0.537</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5676,10 +5676,10 @@
         <v>0.146</v>
       </c>
       <c r="I10">
-        <v>0.049</v>
+        <v>0.054</v>
       </c>
       <c r="J10">
-        <v>0.961</v>
+        <v>0.957</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5708,10 +5708,10 @@
         <v>5.238</v>
       </c>
       <c r="I11">
-        <v>1.796</v>
+        <v>1.148</v>
       </c>
       <c r="J11">
-        <v>0.075</v>
+        <v>0.251</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5740,10 +5740,10 @@
         <v>6.52</v>
       </c>
       <c r="I12">
-        <v>2.296</v>
+        <v>2.038</v>
       </c>
       <c r="J12">
-        <v>0.023</v>
+        <v>0.042</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5772,10 +5772,10 @@
         <v>2.629</v>
       </c>
       <c r="I13">
-        <v>0.887</v>
+        <v>0.738</v>
       </c>
       <c r="J13">
-        <v>0.377</v>
+        <v>0.461</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5804,10 +5804,10 @@
         <v>-0.044</v>
       </c>
       <c r="I14">
-        <v>-1.149</v>
+        <v>-0.886</v>
       </c>
       <c r="J14">
-        <v>0.253</v>
+        <v>0.376</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5836,10 +5836,10 @@
         <v>-0.077</v>
       </c>
       <c r="I15">
-        <v>-1.868</v>
+        <v>-1.389</v>
       </c>
       <c r="J15">
-        <v>0.064</v>
+        <v>0.165</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5868,10 +5868,10 @@
         <v>-0.01</v>
       </c>
       <c r="I16">
-        <v>-0.222</v>
+        <v>-0.191</v>
       </c>
       <c r="J16">
-        <v>0.825</v>
+        <v>0.849</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5900,10 +5900,10 @@
         <v>-0.077</v>
       </c>
       <c r="I17">
-        <v>-1.627</v>
+        <v>-1.278</v>
       </c>
       <c r="J17">
-        <v>0.106</v>
+        <v>0.201</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5932,10 +5932,10 @@
         <v>-0.01</v>
       </c>
       <c r="I18">
-        <v>-0.185</v>
+        <v>-0.216</v>
       </c>
       <c r="J18">
-        <v>0.853</v>
+        <v>0.829</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5964,10 +5964,10 @@
         <v>-0.011</v>
       </c>
       <c r="I19">
-        <v>-0.208</v>
+        <v>-0.257</v>
       </c>
       <c r="J19">
-        <v>0.836</v>
+        <v>0.797</v>
       </c>
     </row>
   </sheetData>
@@ -6046,10 +6046,10 @@
         <v>3.601</v>
       </c>
       <c r="H2">
-        <v>0.923</v>
+        <v>0.646</v>
       </c>
       <c r="I2">
-        <v>0.358</v>
+        <v>0.518</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -6075,10 +6075,10 @@
         <v>2.474</v>
       </c>
       <c r="H3">
-        <v>0.713</v>
+        <v>0.578</v>
       </c>
       <c r="I3">
-        <v>0.477</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -6104,10 +6104,10 @@
         <v>2.292</v>
       </c>
       <c r="H4">
-        <v>0.546</v>
+        <v>0.503</v>
       </c>
       <c r="I4">
-        <v>0.586</v>
+        <v>0.615</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -6133,10 +6133,10 @@
         <v>-2.54</v>
       </c>
       <c r="H5">
-        <v>-0.6</v>
+        <v>-0.721</v>
       </c>
       <c r="I5">
-        <v>0.549</v>
+        <v>0.471</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -6162,10 +6162,10 @@
         <v>-6.8</v>
       </c>
       <c r="H6">
-        <v>-1.546</v>
+        <v>-1.311</v>
       </c>
       <c r="I6">
-        <v>0.124</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -6191,10 +6191,10 @@
         <v>-7.115</v>
       </c>
       <c r="H7">
-        <v>-1.382</v>
+        <v>-1.795</v>
       </c>
       <c r="I7">
-        <v>0.169</v>
+        <v>0.073</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -6220,10 +6220,10 @@
         <v>-1.054</v>
       </c>
       <c r="H8">
-        <v>-0.609</v>
+        <v>-0.47</v>
       </c>
       <c r="I8">
-        <v>0.544</v>
+        <v>0.638</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -6249,10 +6249,10 @@
         <v>-1.506</v>
       </c>
       <c r="H9">
-        <v>-0.953</v>
+        <v>-0.761</v>
       </c>
       <c r="I9">
-        <v>0.342</v>
+        <v>0.447</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -6278,10 +6278,10 @@
         <v>-1.886</v>
       </c>
       <c r="H10">
-        <v>-1.033</v>
+        <v>-0.9399999999999999</v>
       </c>
       <c r="I10">
-        <v>0.304</v>
+        <v>0.347</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -6307,10 +6307,10 @@
         <v>1.045</v>
       </c>
       <c r="H11">
-        <v>0.549</v>
+        <v>0.61</v>
       </c>
       <c r="I11">
-        <v>0.584</v>
+        <v>0.542</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -6336,10 +6336,10 @@
         <v>2.819</v>
       </c>
       <c r="H12">
-        <v>1.506</v>
+        <v>1.2</v>
       </c>
       <c r="I12">
-        <v>0.134</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -6365,10 +6365,10 @@
         <v>1.859</v>
       </c>
       <c r="H13">
-        <v>0.988</v>
+        <v>1.206</v>
       </c>
       <c r="I13">
-        <v>0.325</v>
+        <v>0.228</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -6394,10 +6394,10 @@
         <v>-0.003</v>
       </c>
       <c r="H14">
-        <v>-0.124</v>
+        <v>-0.146</v>
       </c>
       <c r="I14">
-        <v>0.902</v>
+        <v>0.884</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -6423,10 +6423,10 @@
         <v>-0.022</v>
       </c>
       <c r="H15">
-        <v>-0.834</v>
+        <v>-0.717</v>
       </c>
       <c r="I15">
-        <v>0.406</v>
+        <v>0.473</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -6452,10 +6452,10 @@
         <v>-0.007</v>
       </c>
       <c r="H16">
-        <v>-0.236</v>
+        <v>-0.166</v>
       </c>
       <c r="I16">
-        <v>0.8139999999999999</v>
+        <v>0.868</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -6481,10 +6481,10 @@
         <v>-0.024</v>
       </c>
       <c r="H17">
-        <v>-0.775</v>
+        <v>-0.6929999999999999</v>
       </c>
       <c r="I17">
-        <v>0.439</v>
+        <v>0.488</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -6510,10 +6510,10 @@
         <v>-0.007</v>
       </c>
       <c r="H18">
-        <v>-0.213</v>
+        <v>-0.148</v>
       </c>
       <c r="I18">
-        <v>0.832</v>
+        <v>0.882</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -6539,10 +6539,10 @@
         <v>0.002</v>
       </c>
       <c r="H19">
-        <v>0.053</v>
+        <v>0.061</v>
       </c>
       <c r="I19">
-        <v>0.958</v>
+        <v>0.951</v>
       </c>
     </row>
   </sheetData>
@@ -6628,10 +6628,10 @@
         <v>6.833</v>
       </c>
       <c r="I2">
-        <v>1.501</v>
+        <v>1.167</v>
       </c>
       <c r="J2">
-        <v>0.136</v>
+        <v>0.243</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -6660,10 +6660,10 @@
         <v>3.184</v>
       </c>
       <c r="I3">
-        <v>0.782</v>
+        <v>0.674</v>
       </c>
       <c r="J3">
-        <v>0.435</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6692,10 +6692,10 @@
         <v>3.692</v>
       </c>
       <c r="I4">
-        <v>0.751</v>
+        <v>0.791</v>
       </c>
       <c r="J4">
-        <v>0.454</v>
+        <v>0.429</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6724,10 +6724,10 @@
         <v>-3.107</v>
       </c>
       <c r="I5">
-        <v>-0.626</v>
+        <v>-0.543</v>
       </c>
       <c r="J5">
-        <v>0.532</v>
+        <v>0.587</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6756,10 +6756,10 @@
         <v>-1.888</v>
       </c>
       <c r="I6">
-        <v>-0.363</v>
+        <v>-0.354</v>
       </c>
       <c r="J6">
-        <v>0.717</v>
+        <v>0.724</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -6788,10 +6788,10 @@
         <v>-3.404</v>
       </c>
       <c r="I7">
-        <v>-0.5610000000000001</v>
+        <v>-0.672</v>
       </c>
       <c r="J7">
-        <v>0.576</v>
+        <v>0.501</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -6820,10 +6820,10 @@
         <v>-2.36</v>
       </c>
       <c r="I8">
-        <v>-1.167</v>
+        <v>-1.051</v>
       </c>
       <c r="J8">
-        <v>0.245</v>
+        <v>0.293</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -6852,10 +6852,10 @@
         <v>-2.156</v>
       </c>
       <c r="I9">
-        <v>-1.165</v>
+        <v>-0.958</v>
       </c>
       <c r="J9">
-        <v>0.246</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -6884,10 +6884,10 @@
         <v>-3.002</v>
       </c>
       <c r="I10">
-        <v>-1.407</v>
+        <v>-1.482</v>
       </c>
       <c r="J10">
-        <v>0.162</v>
+        <v>0.138</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -6916,10 +6916,10 @@
         <v>1.69</v>
       </c>
       <c r="I11">
-        <v>0.757</v>
+        <v>0.605</v>
       </c>
       <c r="J11">
-        <v>0.45</v>
+        <v>0.545</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -6948,10 +6948,10 @@
         <v>1.125</v>
       </c>
       <c r="I12">
-        <v>0.509</v>
+        <v>0.5</v>
       </c>
       <c r="J12">
-        <v>0.612</v>
+        <v>0.617</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -6980,10 +6980,10 @@
         <v>0.08</v>
       </c>
       <c r="I13">
-        <v>0.036</v>
+        <v>0.039</v>
       </c>
       <c r="J13">
-        <v>0.971</v>
+        <v>0.969</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -7012,10 +7012,10 @@
         <v>-0.011</v>
       </c>
       <c r="I14">
-        <v>-0.391</v>
+        <v>-0.544</v>
       </c>
       <c r="J14">
-        <v>0.697</v>
+        <v>0.586</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -7044,10 +7044,10 @@
         <v>-0.045</v>
       </c>
       <c r="I15">
-        <v>-1.453</v>
+        <v>-1.534</v>
       </c>
       <c r="J15">
-        <v>0.149</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -7076,10 +7076,10 @@
         <v>-0.024</v>
       </c>
       <c r="I16">
-        <v>-0.718</v>
+        <v>-0.615</v>
       </c>
       <c r="J16">
-        <v>0.474</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -7108,10 +7108,10 @@
         <v>-0.07199999999999999</v>
       </c>
       <c r="I17">
-        <v>-2.056</v>
+        <v>-1.737</v>
       </c>
       <c r="J17">
-        <v>0.042</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -7140,10 +7140,10 @@
         <v>-0.038</v>
       </c>
       <c r="I18">
-        <v>-1.028</v>
+        <v>-0.877</v>
       </c>
       <c r="J18">
-        <v>0.306</v>
+        <v>0.381</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7172,10 +7172,10 @@
         <v>0.025</v>
       </c>
       <c r="I19">
-        <v>0.615</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="J19">
-        <v>0.539</v>
+        <v>0.494</v>
       </c>
     </row>
   </sheetData>
@@ -7261,10 +7261,10 @@
         <v>6.922</v>
       </c>
       <c r="I2">
-        <v>1.264</v>
+        <v>0.985</v>
       </c>
       <c r="J2">
-        <v>0.209</v>
+        <v>0.324</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -7293,10 +7293,10 @@
         <v>0.71</v>
       </c>
       <c r="I3">
-        <v>0.145</v>
+        <v>0.133</v>
       </c>
       <c r="J3">
-        <v>0.885</v>
+        <v>0.894</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -7325,10 +7325,10 @@
         <v>-1.381</v>
       </c>
       <c r="I4">
-        <v>-0.233</v>
+        <v>-0.269</v>
       </c>
       <c r="J4">
-        <v>0.8159999999999999</v>
+        <v>0.788</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -7357,10 +7357,10 @@
         <v>-7.971</v>
       </c>
       <c r="I5">
-        <v>-1.345</v>
+        <v>-1.163</v>
       </c>
       <c r="J5">
-        <v>0.181</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -7389,10 +7389,10 @@
         <v>-3.835</v>
       </c>
       <c r="I6">
-        <v>-0.615</v>
+        <v>-0.5669999999999999</v>
       </c>
       <c r="J6">
-        <v>0.54</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -7421,10 +7421,10 @@
         <v>-11.213</v>
       </c>
       <c r="I7">
-        <v>-1.55</v>
+        <v>-1.62</v>
       </c>
       <c r="J7">
-        <v>0.124</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -7453,10 +7453,10 @@
         <v>-2.827</v>
       </c>
       <c r="I8">
-        <v>-1.164</v>
+        <v>-1.015</v>
       </c>
       <c r="J8">
-        <v>0.246</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -7485,10 +7485,10 @@
         <v>-0.633</v>
       </c>
       <c r="I9">
-        <v>-0.284</v>
+        <v>-0.27</v>
       </c>
       <c r="J9">
-        <v>0.777</v>
+        <v>0.787</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -7517,10 +7517,10 @@
         <v>-0.207</v>
       </c>
       <c r="I10">
-        <v>-0.08</v>
+        <v>-0.095</v>
       </c>
       <c r="J10">
-        <v>0.9360000000000001</v>
+        <v>0.924</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -7549,10 +7549,10 @@
         <v>3.698</v>
       </c>
       <c r="I11">
-        <v>1.388</v>
+        <v>1.13</v>
       </c>
       <c r="J11">
-        <v>0.168</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -7581,10 +7581,10 @@
         <v>2.002</v>
       </c>
       <c r="I12">
-        <v>0.755</v>
+        <v>0.694</v>
       </c>
       <c r="J12">
-        <v>0.452</v>
+        <v>0.488</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -7613,7 +7613,7 @@
         <v>2.83</v>
       </c>
       <c r="I13">
-        <v>1.069</v>
+        <v>1.064</v>
       </c>
       <c r="J13">
         <v>0.287</v>
@@ -7645,10 +7645,10 @@
         <v>-0.034</v>
       </c>
       <c r="I14">
-        <v>-0.981</v>
+        <v>-1.259</v>
       </c>
       <c r="J14">
-        <v>0.328</v>
+        <v>0.208</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -7677,10 +7677,10 @@
         <v>-0.068</v>
       </c>
       <c r="I15">
-        <v>-1.87</v>
+        <v>-1.6</v>
       </c>
       <c r="J15">
-        <v>0.064</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -7741,10 +7741,10 @@
         <v>-0.058</v>
       </c>
       <c r="I17">
-        <v>-1.367</v>
+        <v>-1.043</v>
       </c>
       <c r="J17">
-        <v>0.174</v>
+        <v>0.297</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -7773,10 +7773,10 @@
         <v>-0.031</v>
       </c>
       <c r="I18">
-        <v>-0.68</v>
+        <v>-0.615</v>
       </c>
       <c r="J18">
-        <v>0.498</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7805,10 +7805,10 @@
         <v>-0.016</v>
       </c>
       <c r="I19">
-        <v>-0.338</v>
+        <v>-0.361</v>
       </c>
       <c r="J19">
-        <v>0.736</v>
+        <v>0.718</v>
       </c>
     </row>
   </sheetData>
@@ -7901,10 +7901,10 @@
         <v>5.913</v>
       </c>
       <c r="J2">
-        <v>1.015</v>
+        <v>0.82</v>
       </c>
       <c r="K2">
-        <v>0.312</v>
+        <v>0.412</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -7936,10 +7936,10 @@
         <v>0.774</v>
       </c>
       <c r="J3">
-        <v>0.149</v>
+        <v>0.131</v>
       </c>
       <c r="K3">
-        <v>0.882</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -7971,10 +7971,10 @@
         <v>-0.861</v>
       </c>
       <c r="J4">
-        <v>-0.137</v>
+        <v>-0.15</v>
       </c>
       <c r="K4">
-        <v>0.891</v>
+        <v>0.881</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -8006,10 +8006,10 @@
         <v>-4.298</v>
       </c>
       <c r="J5">
-        <v>-0.68</v>
+        <v>-0.582</v>
       </c>
       <c r="K5">
-        <v>0.498</v>
+        <v>0.5610000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -8041,10 +8041,10 @@
         <v>-8.005000000000001</v>
       </c>
       <c r="J6">
-        <v>-1.214</v>
+        <v>-1.315</v>
       </c>
       <c r="K6">
-        <v>0.227</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -8076,10 +8076,10 @@
         <v>-6.641</v>
       </c>
       <c r="J7">
-        <v>-0.859</v>
+        <v>-1.011</v>
       </c>
       <c r="K7">
-        <v>0.392</v>
+        <v>0.312</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -8111,10 +8111,10 @@
         <v>-1.727</v>
       </c>
       <c r="J8">
-        <v>-0.668</v>
+        <v>-0.527</v>
       </c>
       <c r="K8">
-        <v>0.505</v>
+        <v>0.598</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -8146,10 +8146,10 @@
         <v>-0.824</v>
       </c>
       <c r="J9">
-        <v>-0.348</v>
+        <v>-0.367</v>
       </c>
       <c r="K9">
-        <v>0.729</v>
+        <v>0.713</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -8181,10 +8181,10 @@
         <v>-0.8100000000000001</v>
       </c>
       <c r="J10">
-        <v>-0.296</v>
+        <v>-0.319</v>
       </c>
       <c r="K10">
-        <v>0.768</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -8216,10 +8216,10 @@
         <v>1.84</v>
       </c>
       <c r="J11">
-        <v>0.646</v>
+        <v>0.513</v>
       </c>
       <c r="K11">
-        <v>0.519</v>
+        <v>0.608</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -8251,10 +8251,10 @@
         <v>4.128</v>
       </c>
       <c r="J12">
-        <v>1.475</v>
+        <v>1.688</v>
       </c>
       <c r="K12">
-        <v>0.143</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -8286,10 +8286,10 @@
         <v>2.002</v>
       </c>
       <c r="J13">
-        <v>0.711</v>
+        <v>0.716</v>
       </c>
       <c r="K13">
-        <v>0.478</v>
+        <v>0.474</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -8321,10 +8321,10 @@
         <v>-0.015</v>
       </c>
       <c r="J14">
-        <v>-0.398</v>
+        <v>-0.397</v>
       </c>
       <c r="K14">
-        <v>0.6909999999999999</v>
+        <v>0.6919999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -8356,10 +8356,10 @@
         <v>-0.043</v>
       </c>
       <c r="J15">
-        <v>-1.095</v>
+        <v>-0.962</v>
       </c>
       <c r="K15">
-        <v>0.276</v>
+        <v>0.336</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -8391,10 +8391,10 @@
         <v>-0.015</v>
       </c>
       <c r="J16">
-        <v>-0.351</v>
+        <v>-0.383</v>
       </c>
       <c r="K16">
-        <v>0.726</v>
+        <v>0.702</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -8426,10 +8426,10 @@
         <v>-0.077</v>
       </c>
       <c r="J17">
-        <v>-1.709</v>
+        <v>-1.774</v>
       </c>
       <c r="K17">
-        <v>0.09</v>
+        <v>0.076</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -8461,10 +8461,10 @@
         <v>-0.03</v>
       </c>
       <c r="J18">
-        <v>-0.621</v>
+        <v>-0.6</v>
       </c>
       <c r="K18">
-        <v>0.536</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -8496,10 +8496,10 @@
         <v>-0.014</v>
       </c>
       <c r="J19">
-        <v>-0.267</v>
+        <v>-0.304</v>
       </c>
       <c r="K19">
-        <v>0.79</v>
+        <v>0.761</v>
       </c>
     </row>
   </sheetData>
@@ -8578,10 +8578,10 @@
         <v>-1.396</v>
       </c>
       <c r="H2">
-        <v>-0.282</v>
+        <v>-0.308</v>
       </c>
       <c r="I2">
-        <v>0.778</v>
+        <v>0.758</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8607,10 +8607,10 @@
         <v>5.141</v>
       </c>
       <c r="H3">
-        <v>1.092</v>
+        <v>1.035</v>
       </c>
       <c r="I3">
-        <v>0.276</v>
+        <v>0.301</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -8636,10 +8636,10 @@
         <v>7.111</v>
       </c>
       <c r="H4">
-        <v>1.329</v>
+        <v>1.114</v>
       </c>
       <c r="I4">
-        <v>0.185</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -8665,10 +8665,10 @@
         <v>-1.61</v>
       </c>
       <c r="H5">
-        <v>-0.312</v>
+        <v>-0.274</v>
       </c>
       <c r="I5">
-        <v>0.755</v>
+        <v>0.784</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -8694,10 +8694,10 @@
         <v>-3.171</v>
       </c>
       <c r="H6">
-        <v>-0.586</v>
+        <v>-0.476</v>
       </c>
       <c r="I6">
-        <v>0.5580000000000001</v>
+        <v>0.634</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -8723,10 +8723,10 @@
         <v>-8.241</v>
       </c>
       <c r="H7">
-        <v>-1.35</v>
+        <v>-1.769</v>
       </c>
       <c r="I7">
-        <v>0.179</v>
+        <v>0.077</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -8752,10 +8752,10 @@
         <v>0.66</v>
       </c>
       <c r="H8">
-        <v>0.311</v>
+        <v>0.318</v>
       </c>
       <c r="I8">
-        <v>0.756</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -8781,10 +8781,10 @@
         <v>-3.266</v>
       </c>
       <c r="H9">
-        <v>-1.605</v>
+        <v>-1.443</v>
       </c>
       <c r="I9">
-        <v>0.11</v>
+        <v>0.149</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -8810,10 +8810,10 @@
         <v>-3.558</v>
       </c>
       <c r="H10">
-        <v>-1.596</v>
+        <v>-1.359</v>
       </c>
       <c r="I10">
-        <v>0.112</v>
+        <v>0.174</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8839,10 +8839,10 @@
         <v>1.459</v>
       </c>
       <c r="H11">
-        <v>0.649</v>
+        <v>0.58</v>
       </c>
       <c r="I11">
-        <v>0.517</v>
+        <v>0.5620000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -8868,10 +8868,10 @@
         <v>1.77</v>
       </c>
       <c r="H12">
-        <v>0.786</v>
+        <v>0.695</v>
       </c>
       <c r="I12">
-        <v>0.433</v>
+        <v>0.487</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -8897,10 +8897,10 @@
         <v>2.12</v>
       </c>
       <c r="H13">
-        <v>0.9409999999999999</v>
+        <v>1.184</v>
       </c>
       <c r="I13">
-        <v>0.348</v>
+        <v>0.236</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -8926,10 +8926,10 @@
         <v>-0.013</v>
       </c>
       <c r="H14">
-        <v>-0.425</v>
+        <v>-0.478</v>
       </c>
       <c r="I14">
-        <v>0.671</v>
+        <v>0.632</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -8955,10 +8955,10 @@
         <v>0.015</v>
       </c>
       <c r="H15">
-        <v>0.492</v>
+        <v>0.359</v>
       </c>
       <c r="I15">
-        <v>0.623</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -8984,10 +8984,10 @@
         <v>0.002</v>
       </c>
       <c r="H16">
-        <v>0.046</v>
+        <v>0.032</v>
       </c>
       <c r="I16">
-        <v>0.963</v>
+        <v>0.975</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -9013,10 +9013,10 @@
         <v>-0.06</v>
       </c>
       <c r="H17">
-        <v>-1.719</v>
+        <v>-1.596</v>
       </c>
       <c r="I17">
-        <v>0.08699999999999999</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -9042,10 +9042,10 @@
         <v>-0.021</v>
       </c>
       <c r="H18">
-        <v>-0.542</v>
+        <v>-0.603</v>
       </c>
       <c r="I18">
-        <v>0.588</v>
+        <v>0.546</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -9071,10 +9071,10 @@
         <v>0.048</v>
       </c>
       <c r="H19">
-        <v>1.116</v>
+        <v>1.141</v>
       </c>
       <c r="I19">
-        <v>0.266</v>
+        <v>0.254</v>
       </c>
     </row>
   </sheetData>
@@ -9153,10 +9153,10 @@
         <v>-0.762</v>
       </c>
       <c r="H2">
-        <v>-0.122</v>
+        <v>-0.12</v>
       </c>
       <c r="I2">
-        <v>0.903</v>
+        <v>0.905</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -9182,10 +9182,10 @@
         <v>2.366</v>
       </c>
       <c r="H3">
-        <v>0.398</v>
+        <v>0.492</v>
       </c>
       <c r="I3">
-        <v>0.6909999999999999</v>
+        <v>0.623</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -9211,10 +9211,10 @@
         <v>7.112</v>
       </c>
       <c r="H4">
-        <v>1.054</v>
+        <v>1.078</v>
       </c>
       <c r="I4">
-        <v>0.293</v>
+        <v>0.281</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -9240,10 +9240,10 @@
         <v>-2.82</v>
       </c>
       <c r="H5">
-        <v>-0.434</v>
+        <v>-0.414</v>
       </c>
       <c r="I5">
-        <v>0.665</v>
+        <v>0.679</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -9269,10 +9269,10 @@
         <v>-6.491</v>
       </c>
       <c r="H6">
-        <v>-0.955</v>
+        <v>-0.723</v>
       </c>
       <c r="I6">
-        <v>0.341</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -9298,10 +9298,10 @@
         <v>-13.555</v>
       </c>
       <c r="H7">
-        <v>-1.771</v>
+        <v>-2.048</v>
       </c>
       <c r="I7">
-        <v>0.078</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -9327,10 +9327,10 @@
         <v>0.138</v>
       </c>
       <c r="H8">
-        <v>0.052</v>
+        <v>0.047</v>
       </c>
       <c r="I8">
-        <v>0.959</v>
+        <v>0.962</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -9356,10 +9356,10 @@
         <v>-2.002</v>
       </c>
       <c r="H9">
-        <v>-0.777</v>
+        <v>-0.893</v>
       </c>
       <c r="I9">
-        <v>0.438</v>
+        <v>0.372</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -9385,10 +9385,10 @@
         <v>-3.232</v>
       </c>
       <c r="H10">
-        <v>-1.148</v>
+        <v>-1.155</v>
       </c>
       <c r="I10">
-        <v>0.253</v>
+        <v>0.248</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -9414,10 +9414,10 @@
         <v>1.514</v>
       </c>
       <c r="H11">
-        <v>0.535</v>
+        <v>0.495</v>
       </c>
       <c r="I11">
-        <v>0.594</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -9443,10 +9443,10 @@
         <v>3.096</v>
       </c>
       <c r="H12">
-        <v>1.095</v>
+        <v>0.959</v>
       </c>
       <c r="I12">
-        <v>0.275</v>
+        <v>0.337</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -9472,10 +9472,10 @@
         <v>3.707</v>
       </c>
       <c r="H13">
-        <v>1.31</v>
+        <v>1.907</v>
       </c>
       <c r="I13">
-        <v>0.192</v>
+        <v>0.057</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -9501,10 +9501,10 @@
         <v>0.002</v>
       </c>
       <c r="H14">
-        <v>0.044</v>
+        <v>0.038</v>
       </c>
       <c r="I14">
-        <v>0.965</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -9530,10 +9530,10 @@
         <v>-0.045</v>
       </c>
       <c r="H15">
-        <v>-1.162</v>
+        <v>-0.996</v>
       </c>
       <c r="I15">
-        <v>0.247</v>
+        <v>0.319</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -9559,10 +9559,10 @@
         <v>0.005</v>
       </c>
       <c r="H16">
-        <v>0.118</v>
+        <v>0.097</v>
       </c>
       <c r="I16">
-        <v>0.907</v>
+        <v>0.923</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -9588,10 +9588,10 @@
         <v>-0.064</v>
       </c>
       <c r="H17">
-        <v>-1.463</v>
+        <v>-1.302</v>
       </c>
       <c r="I17">
-        <v>0.145</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -9617,10 +9617,10 @@
         <v>-0.051</v>
       </c>
       <c r="H18">
-        <v>-1.045</v>
+        <v>-0.974</v>
       </c>
       <c r="I18">
-        <v>0.298</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -9646,10 +9646,10 @@
         <v>0.015</v>
       </c>
       <c r="H19">
-        <v>0.275</v>
+        <v>0.295</v>
       </c>
       <c r="I19">
-        <v>0.783</v>
+        <v>0.768</v>
       </c>
     </row>
   </sheetData>
@@ -9735,10 +9735,10 @@
         <v>-0.342</v>
       </c>
       <c r="I2">
-        <v>-0.046</v>
+        <v>-0.036</v>
       </c>
       <c r="J2">
-        <v>0.963</v>
+        <v>0.972</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9767,10 +9767,10 @@
         <v>0.105</v>
       </c>
       <c r="I3">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
       <c r="J3">
-        <v>0.988</v>
+        <v>0.986</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9799,10 +9799,10 @@
         <v>7.032</v>
       </c>
       <c r="I4">
-        <v>0.876</v>
+        <v>1.01</v>
       </c>
       <c r="J4">
-        <v>0.382</v>
+        <v>0.312</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -9831,10 +9831,10 @@
         <v>0.497</v>
       </c>
       <c r="I5">
-        <v>0.064</v>
+        <v>0.05</v>
       </c>
       <c r="J5">
-        <v>0.949</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9863,10 +9863,10 @@
         <v>-1.225</v>
       </c>
       <c r="I6">
-        <v>-0.151</v>
+        <v>-0.123</v>
       </c>
       <c r="J6">
-        <v>0.88</v>
+        <v>0.902</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -9895,10 +9895,10 @@
         <v>-8.800000000000001</v>
       </c>
       <c r="I7">
-        <v>-0.961</v>
+        <v>-0.974</v>
       </c>
       <c r="J7">
-        <v>0.338</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -9927,10 +9927,10 @@
         <v>-0.031</v>
       </c>
       <c r="I8">
-        <v>-0.01</v>
+        <v>-0.007</v>
       </c>
       <c r="J8">
-        <v>0.992</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9959,10 +9959,10 @@
         <v>-0.427</v>
       </c>
       <c r="I9">
-        <v>-0.139</v>
+        <v>-0.162</v>
       </c>
       <c r="J9">
-        <v>0.89</v>
+        <v>0.872</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9991,10 +9991,10 @@
         <v>-2.372</v>
       </c>
       <c r="I10">
-        <v>-0.707</v>
+        <v>-0.736</v>
       </c>
       <c r="J10">
-        <v>0.481</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10023,10 +10023,10 @@
         <v>-0.128</v>
       </c>
       <c r="I11">
-        <v>-0.038</v>
+        <v>-0.028</v>
       </c>
       <c r="J11">
-        <v>0.97</v>
+        <v>0.977</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -10055,10 +10055,10 @@
         <v>0.877</v>
       </c>
       <c r="I12">
-        <v>0.26</v>
+        <v>0.244</v>
       </c>
       <c r="J12">
-        <v>0.795</v>
+        <v>0.8070000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -10087,10 +10087,10 @@
         <v>2.284</v>
       </c>
       <c r="I13">
-        <v>0.676</v>
+        <v>0.772</v>
       </c>
       <c r="J13">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -10151,10 +10151,10 @@
         <v>-0.04</v>
       </c>
       <c r="I15">
-        <v>-0.867</v>
+        <v>-0.751</v>
       </c>
       <c r="J15">
-        <v>0.387</v>
+        <v>0.452</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -10183,10 +10183,10 @@
         <v>-0.034</v>
       </c>
       <c r="I16">
-        <v>-0.658</v>
+        <v>-0.481</v>
       </c>
       <c r="J16">
-        <v>0.511</v>
+        <v>0.631</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -10215,7 +10215,7 @@
         <v>-0.045</v>
       </c>
       <c r="I17">
-        <v>-0.851</v>
+        <v>-0.848</v>
       </c>
       <c r="J17">
         <v>0.396</v>
@@ -10247,10 +10247,10 @@
         <v>-0.019</v>
       </c>
       <c r="I18">
-        <v>-0.322</v>
+        <v>-0.319</v>
       </c>
       <c r="J18">
-        <v>0.748</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -10279,10 +10279,10 @@
         <v>-0.006</v>
       </c>
       <c r="I19">
-        <v>-0.099</v>
+        <v>-0.108</v>
       </c>
       <c r="J19">
-        <v>0.921</v>
+        <v>0.914</v>
       </c>
     </row>
   </sheetData>
@@ -10361,10 +10361,10 @@
         <v>-0.9</v>
       </c>
       <c r="H2">
-        <v>-0.217</v>
+        <v>-0.196</v>
       </c>
       <c r="I2">
-        <v>0.828</v>
+        <v>0.845</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -10390,10 +10390,10 @@
         <v>1.167</v>
       </c>
       <c r="H3">
-        <v>0.304</v>
+        <v>0.267</v>
       </c>
       <c r="I3">
-        <v>0.762</v>
+        <v>0.789</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -10419,10 +10419,10 @@
         <v>2.433</v>
       </c>
       <c r="H4">
-        <v>0.549</v>
+        <v>0.591</v>
       </c>
       <c r="I4">
-        <v>0.583</v>
+        <v>0.555</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -10448,10 +10448,10 @@
         <v>-1.397</v>
       </c>
       <c r="H5">
-        <v>-0.332</v>
+        <v>-0.342</v>
       </c>
       <c r="I5">
-        <v>0.741</v>
+        <v>0.733</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -10477,10 +10477,10 @@
         <v>-6.934</v>
       </c>
       <c r="H6">
-        <v>-1.58</v>
+        <v>-1.468</v>
       </c>
       <c r="I6">
-        <v>0.116</v>
+        <v>0.142</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -10506,10 +10506,10 @@
         <v>-6.867</v>
       </c>
       <c r="H7">
-        <v>-1.357</v>
+        <v>-1.498</v>
       </c>
       <c r="I7">
-        <v>0.177</v>
+        <v>0.134</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -10535,10 +10535,10 @@
         <v>0.781</v>
       </c>
       <c r="H8">
-        <v>0.441</v>
+        <v>0.403</v>
       </c>
       <c r="I8">
-        <v>0.66</v>
+        <v>0.6870000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -10564,10 +10564,10 @@
         <v>-0.469</v>
       </c>
       <c r="H9">
-        <v>-0.28</v>
+        <v>-0.243</v>
       </c>
       <c r="I9">
-        <v>0.78</v>
+        <v>0.8080000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -10593,10 +10593,10 @@
         <v>-1.488</v>
       </c>
       <c r="H10">
-        <v>-0.8</v>
+        <v>-0.792</v>
       </c>
       <c r="I10">
-        <v>0.425</v>
+        <v>0.428</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -10622,10 +10622,10 @@
         <v>0.857</v>
       </c>
       <c r="H11">
-        <v>0.458</v>
+        <v>0.444</v>
       </c>
       <c r="I11">
-        <v>0.648</v>
+        <v>0.657</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -10651,10 +10651,10 @@
         <v>2.837</v>
       </c>
       <c r="H12">
-        <v>1.548</v>
+        <v>1.388</v>
       </c>
       <c r="I12">
-        <v>0.124</v>
+        <v>0.165</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -10680,10 +10680,10 @@
         <v>2.599</v>
       </c>
       <c r="H13">
-        <v>1.391</v>
+        <v>1.65</v>
       </c>
       <c r="I13">
-        <v>0.166</v>
+        <v>0.099</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -10709,10 +10709,10 @@
         <v>-0.015</v>
       </c>
       <c r="H14">
-        <v>-0.608</v>
+        <v>-0.755</v>
       </c>
       <c r="I14">
-        <v>0.544</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -10738,10 +10738,10 @@
         <v>-0.034</v>
       </c>
       <c r="H15">
-        <v>-1.298</v>
+        <v>-1.108</v>
       </c>
       <c r="I15">
-        <v>0.196</v>
+        <v>0.268</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -10767,10 +10767,10 @@
         <v>-0.024</v>
       </c>
       <c r="H16">
-        <v>-0.869</v>
+        <v>-0.6</v>
       </c>
       <c r="I16">
-        <v>0.386</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -10796,10 +10796,10 @@
         <v>-0.034</v>
       </c>
       <c r="H17">
-        <v>-1.159</v>
+        <v>-1.506</v>
       </c>
       <c r="I17">
-        <v>0.248</v>
+        <v>0.132</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -10825,10 +10825,10 @@
         <v>-0.004</v>
       </c>
       <c r="H18">
-        <v>-0.136</v>
+        <v>-0.127</v>
       </c>
       <c r="I18">
-        <v>0.892</v>
+        <v>0.899</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -10854,10 +10854,10 @@
         <v>0.032</v>
       </c>
       <c r="H19">
-        <v>0.903</v>
+        <v>1.078</v>
       </c>
       <c r="I19">
-        <v>0.368</v>
+        <v>0.281</v>
       </c>
     </row>
   </sheetData>
@@ -10936,10 +10936,10 @@
         <v>-0.609</v>
       </c>
       <c r="H2">
-        <v>-0.121</v>
+        <v>-0.124</v>
       </c>
       <c r="I2">
-        <v>0.904</v>
+        <v>0.901</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -10965,10 +10965,10 @@
         <v>3.283</v>
       </c>
       <c r="H3">
-        <v>0.702</v>
+        <v>0.492</v>
       </c>
       <c r="I3">
-        <v>0.484</v>
+        <v>0.623</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -10994,10 +10994,10 @@
         <v>4.595</v>
       </c>
       <c r="H4">
-        <v>0.853</v>
+        <v>0.754</v>
       </c>
       <c r="I4">
-        <v>0.395</v>
+        <v>0.451</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -11023,10 +11023,10 @@
         <v>-5.865</v>
       </c>
       <c r="H5">
-        <v>-1.147</v>
+        <v>-0.9360000000000001</v>
       </c>
       <c r="I5">
-        <v>0.253</v>
+        <v>0.349</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -11052,10 +11052,10 @@
         <v>-8.223000000000001</v>
       </c>
       <c r="H6">
-        <v>-1.537</v>
+        <v>-1.561</v>
       </c>
       <c r="I6">
-        <v>0.126</v>
+        <v>0.118</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -11081,10 +11081,10 @@
         <v>-9.801</v>
       </c>
       <c r="H7">
-        <v>-1.593</v>
+        <v>-1.597</v>
       </c>
       <c r="I7">
-        <v>0.113</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -11110,10 +11110,10 @@
         <v>1.021</v>
       </c>
       <c r="H8">
-        <v>0.473</v>
+        <v>0.527</v>
       </c>
       <c r="I8">
-        <v>0.637</v>
+        <v>0.598</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -11139,10 +11139,10 @@
         <v>-1.99</v>
       </c>
       <c r="H9">
-        <v>-0.976</v>
+        <v>-0.6860000000000001</v>
       </c>
       <c r="I9">
-        <v>0.331</v>
+        <v>0.493</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -11168,10 +11168,10 @@
         <v>-2.684</v>
       </c>
       <c r="H10">
-        <v>-1.188</v>
+        <v>-1.091</v>
       </c>
       <c r="I10">
-        <v>0.237</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -11197,10 +11197,10 @@
         <v>2.796</v>
       </c>
       <c r="H11">
-        <v>1.232</v>
+        <v>0.983</v>
       </c>
       <c r="I11">
-        <v>0.22</v>
+        <v>0.326</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -11226,10 +11226,10 @@
         <v>3.678</v>
       </c>
       <c r="H12">
-        <v>1.648</v>
+        <v>1.678</v>
       </c>
       <c r="I12">
-        <v>0.101</v>
+        <v>0.093</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -11255,10 +11255,10 @@
         <v>2.981</v>
       </c>
       <c r="H13">
-        <v>1.308</v>
+        <v>1.264</v>
       </c>
       <c r="I13">
-        <v>0.193</v>
+        <v>0.206</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -11284,10 +11284,10 @@
         <v>-0.058</v>
       </c>
       <c r="H14">
-        <v>-1.895</v>
+        <v>-2.034</v>
       </c>
       <c r="I14">
-        <v>0.06</v>
+        <v>0.042</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -11313,10 +11313,10 @@
         <v>-0.07099999999999999</v>
       </c>
       <c r="H15">
-        <v>-2.268</v>
+        <v>-1.764</v>
       </c>
       <c r="I15">
-        <v>0.025</v>
+        <v>0.078</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -11342,10 +11342,10 @@
         <v>-0.049</v>
       </c>
       <c r="H16">
-        <v>-1.434</v>
+        <v>-1.257</v>
       </c>
       <c r="I16">
-        <v>0.153</v>
+        <v>0.209</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -11371,10 +11371,10 @@
         <v>-0.08599999999999999</v>
       </c>
       <c r="H17">
-        <v>-2.419</v>
+        <v>-2.201</v>
       </c>
       <c r="I17">
-        <v>0.017</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -11400,10 +11400,10 @@
         <v>-0.014</v>
       </c>
       <c r="H18">
-        <v>-0.355</v>
+        <v>-0.482</v>
       </c>
       <c r="I18">
-        <v>0.723</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -11429,10 +11429,10 @@
         <v>0.051</v>
       </c>
       <c r="H19">
-        <v>1.179</v>
+        <v>1.378</v>
       </c>
       <c r="I19">
-        <v>0.24</v>
+        <v>0.168</v>
       </c>
     </row>
   </sheetData>
@@ -11518,10 +11518,10 @@
         <v>1.995</v>
       </c>
       <c r="I2">
-        <v>0.347</v>
+        <v>0.316</v>
       </c>
       <c r="J2">
-        <v>0.729</v>
+        <v>0.752</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11550,10 +11550,10 @@
         <v>1.474</v>
       </c>
       <c r="I3">
-        <v>0.276</v>
+        <v>0.243</v>
       </c>
       <c r="J3">
-        <v>0.783</v>
+        <v>0.8080000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11582,10 +11582,10 @@
         <v>0.819</v>
       </c>
       <c r="I4">
-        <v>0.133</v>
+        <v>0.114</v>
       </c>
       <c r="J4">
-        <v>0.894</v>
+        <v>0.909</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -11614,10 +11614,10 @@
         <v>-7.739</v>
       </c>
       <c r="I5">
-        <v>-1.329</v>
+        <v>-1.307</v>
       </c>
       <c r="J5">
-        <v>0.186</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11646,10 +11646,10 @@
         <v>-10.614</v>
       </c>
       <c r="I6">
-        <v>-1.744</v>
+        <v>-1.474</v>
       </c>
       <c r="J6">
-        <v>0.083</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -11678,10 +11678,10 @@
         <v>-16.856</v>
       </c>
       <c r="I7">
-        <v>-2.428</v>
+        <v>-2.306</v>
       </c>
       <c r="J7">
-        <v>0.016</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -11710,10 +11710,10 @@
         <v>-0.27</v>
       </c>
       <c r="I8">
-        <v>-0.11</v>
+        <v>-0.108</v>
       </c>
       <c r="J8">
-        <v>0.913</v>
+        <v>0.914</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11742,10 +11742,10 @@
         <v>-0.736</v>
       </c>
       <c r="I9">
-        <v>-0.316</v>
+        <v>-0.274</v>
       </c>
       <c r="J9">
-        <v>0.752</v>
+        <v>0.784</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11774,10 +11774,10 @@
         <v>-0.547</v>
       </c>
       <c r="I10">
-        <v>-0.211</v>
+        <v>-0.177</v>
       </c>
       <c r="J10">
-        <v>0.833</v>
+        <v>0.859</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11806,10 +11806,10 @@
         <v>3.73</v>
       </c>
       <c r="I11">
-        <v>1.444</v>
+        <v>1.386</v>
       </c>
       <c r="J11">
-        <v>0.151</v>
+        <v>0.166</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -11838,10 +11838,10 @@
         <v>4.676</v>
       </c>
       <c r="I12">
-        <v>1.843</v>
+        <v>1.608</v>
       </c>
       <c r="J12">
-        <v>0.067</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -11870,10 +11870,10 @@
         <v>5.23</v>
       </c>
       <c r="I13">
-        <v>2.028</v>
+        <v>2.198</v>
       </c>
       <c r="J13">
-        <v>0.044</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -11902,10 +11902,10 @@
         <v>-0.081</v>
       </c>
       <c r="I14">
-        <v>-2.354</v>
+        <v>-2.465</v>
       </c>
       <c r="J14">
-        <v>0.02</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -11934,10 +11934,10 @@
         <v>-0.113</v>
       </c>
       <c r="I15">
-        <v>-3.216</v>
+        <v>-2.113</v>
       </c>
       <c r="J15">
-        <v>0.002</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -11966,10 +11966,10 @@
         <v>-0.061</v>
       </c>
       <c r="I16">
-        <v>-1.572</v>
+        <v>-1.536</v>
       </c>
       <c r="J16">
-        <v>0.118</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -11998,10 +11998,10 @@
         <v>-0.104</v>
       </c>
       <c r="I17">
-        <v>-2.56</v>
+        <v>-2.34</v>
       </c>
       <c r="J17">
-        <v>0.011</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -12030,10 +12030,10 @@
         <v>-0.03</v>
       </c>
       <c r="I18">
-        <v>-0.655</v>
+        <v>-0.635</v>
       </c>
       <c r="J18">
-        <v>0.514</v>
+        <v>0.526</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -12062,10 +12062,10 @@
         <v>0.014</v>
       </c>
       <c r="I19">
-        <v>0.284</v>
+        <v>0.262</v>
       </c>
       <c r="J19">
-        <v>0.776</v>
+        <v>0.793</v>
       </c>
     </row>
   </sheetData>
@@ -12154,7 +12154,7 @@
         <v>-0.089</v>
       </c>
       <c r="J2">
-        <v>0.93</v>
+        <v>0.929</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12183,10 +12183,10 @@
         <v>0.165</v>
       </c>
       <c r="I3">
-        <v>0.026</v>
+        <v>0.02</v>
       </c>
       <c r="J3">
-        <v>0.979</v>
+        <v>0.984</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12218,7 +12218,7 @@
         <v>-0.011</v>
       </c>
       <c r="J4">
-        <v>0.991</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -12247,10 +12247,10 @@
         <v>-5.504</v>
       </c>
       <c r="I5">
-        <v>-0.788</v>
+        <v>-0.652</v>
       </c>
       <c r="J5">
-        <v>0.432</v>
+        <v>0.514</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12279,10 +12279,10 @@
         <v>-9.183</v>
       </c>
       <c r="I6">
-        <v>-1.257</v>
+        <v>-1.133</v>
       </c>
       <c r="J6">
-        <v>0.211</v>
+        <v>0.257</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -12311,10 +12311,10 @@
         <v>-13.189</v>
       </c>
       <c r="I7">
-        <v>-1.573</v>
+        <v>-1.369</v>
       </c>
       <c r="J7">
-        <v>0.118</v>
+        <v>0.171</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -12343,10 +12343,10 @@
         <v>1.169</v>
       </c>
       <c r="I8">
-        <v>0.397</v>
+        <v>0.421</v>
       </c>
       <c r="J8">
-        <v>0.6919999999999999</v>
+        <v>0.674</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12375,10 +12375,10 @@
         <v>0.355</v>
       </c>
       <c r="I9">
-        <v>0.127</v>
+        <v>0.099</v>
       </c>
       <c r="J9">
-        <v>0.899</v>
+        <v>0.921</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12407,10 +12407,10 @@
         <v>-0.027</v>
       </c>
       <c r="I10">
-        <v>-0.008999999999999999</v>
+        <v>-0.008</v>
       </c>
       <c r="J10">
-        <v>0.993</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12439,10 +12439,10 @@
         <v>2.695</v>
       </c>
       <c r="I11">
-        <v>0.869</v>
+        <v>0.642</v>
       </c>
       <c r="J11">
-        <v>0.386</v>
+        <v>0.521</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -12471,10 +12471,10 @@
         <v>3.596</v>
       </c>
       <c r="I12">
-        <v>1.178</v>
+        <v>1.082</v>
       </c>
       <c r="J12">
-        <v>0.241</v>
+        <v>0.279</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -12503,10 +12503,10 @@
         <v>4.054</v>
       </c>
       <c r="I13">
-        <v>1.305</v>
+        <v>1.229</v>
       </c>
       <c r="J13">
-        <v>0.194</v>
+        <v>0.219</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -12535,10 +12535,10 @@
         <v>-0.08400000000000001</v>
       </c>
       <c r="I14">
-        <v>-2.017</v>
+        <v>-1.743</v>
       </c>
       <c r="J14">
-        <v>0.045</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -12567,10 +12567,10 @@
         <v>-0.125</v>
       </c>
       <c r="I15">
-        <v>-2.951</v>
+        <v>-1.895</v>
       </c>
       <c r="J15">
-        <v>0.004</v>
+        <v>0.058</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -12599,10 +12599,10 @@
         <v>-0.089</v>
       </c>
       <c r="I16">
-        <v>-1.933</v>
+        <v>-1.587</v>
       </c>
       <c r="J16">
-        <v>0.055</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -12631,10 +12631,10 @@
         <v>-0.099</v>
       </c>
       <c r="I17">
-        <v>-2.026</v>
+        <v>-1.947</v>
       </c>
       <c r="J17">
-        <v>0.044</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -12663,10 +12663,10 @@
         <v>0.001</v>
       </c>
       <c r="I18">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="J18">
-        <v>0.982</v>
+        <v>0.979</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -12695,10 +12695,10 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="I19">
-        <v>0.144</v>
+        <v>0.181</v>
       </c>
       <c r="J19">
-        <v>0.886</v>
+        <v>0.856</v>
       </c>
     </row>
   </sheetData>
@@ -12777,10 +12777,10 @@
         <v>4.954</v>
       </c>
       <c r="H2">
-        <v>1.161</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="I2">
-        <v>0.247</v>
+        <v>0.416</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -12806,10 +12806,10 @@
         <v>3.494</v>
       </c>
       <c r="H3">
-        <v>0.889</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="I3">
-        <v>0.375</v>
+        <v>0.489</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -12835,10 +12835,10 @@
         <v>7.586</v>
       </c>
       <c r="H4">
-        <v>1.64</v>
+        <v>1.472</v>
       </c>
       <c r="I4">
-        <v>0.103</v>
+        <v>0.141</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -12864,10 +12864,10 @@
         <v>-1.57</v>
       </c>
       <c r="H5">
-        <v>-0.356</v>
+        <v>-0.39</v>
       </c>
       <c r="I5">
-        <v>0.722</v>
+        <v>0.697</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -12893,10 +12893,10 @@
         <v>-7.51</v>
       </c>
       <c r="H6">
-        <v>-1.665</v>
+        <v>-1.197</v>
       </c>
       <c r="I6">
-        <v>0.098</v>
+        <v>0.231</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -12922,10 +12922,10 @@
         <v>-7.458</v>
       </c>
       <c r="H7">
-        <v>-1.377</v>
+        <v>-1.159</v>
       </c>
       <c r="I7">
-        <v>0.171</v>
+        <v>0.246</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -12951,10 +12951,10 @@
         <v>-2.034</v>
       </c>
       <c r="H8">
-        <v>-1.087</v>
+        <v>-0.823</v>
       </c>
       <c r="I8">
-        <v>0.279</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -12980,10 +12980,10 @@
         <v>-2.122</v>
       </c>
       <c r="H9">
-        <v>-1.219</v>
+        <v>-0.984</v>
       </c>
       <c r="I9">
-        <v>0.225</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -13009,10 +13009,10 @@
         <v>-3.584</v>
       </c>
       <c r="H10">
-        <v>-1.828</v>
+        <v>-1.543</v>
       </c>
       <c r="I10">
-        <v>0.07000000000000001</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -13038,10 +13038,10 @@
         <v>0.536</v>
       </c>
       <c r="H11">
-        <v>0.27</v>
+        <v>0.267</v>
       </c>
       <c r="I11">
-        <v>0.787</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -13067,10 +13067,10 @@
         <v>3.205</v>
       </c>
       <c r="H12">
-        <v>1.664</v>
+        <v>1.18</v>
       </c>
       <c r="I12">
-        <v>0.098</v>
+        <v>0.238</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -13096,10 +13096,10 @@
         <v>2.164</v>
       </c>
       <c r="H13">
-        <v>1.086</v>
+        <v>1.002</v>
       </c>
       <c r="I13">
-        <v>0.279</v>
+        <v>0.317</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -13125,10 +13125,10 @@
         <v>-0.003</v>
       </c>
       <c r="H14">
-        <v>-0.098</v>
+        <v>-0.093</v>
       </c>
       <c r="I14">
-        <v>0.922</v>
+        <v>0.926</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -13154,10 +13154,10 @@
         <v>-0.036</v>
       </c>
       <c r="H15">
-        <v>-1.283</v>
+        <v>-0.951</v>
       </c>
       <c r="I15">
-        <v>0.201</v>
+        <v>0.341</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -13183,10 +13183,10 @@
         <v>-0.005</v>
       </c>
       <c r="H16">
-        <v>-0.159</v>
+        <v>-0.1</v>
       </c>
       <c r="I16">
-        <v>0.874</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -13212,10 +13212,10 @@
         <v>-0.035</v>
       </c>
       <c r="H17">
-        <v>-1.082</v>
+        <v>-1.167</v>
       </c>
       <c r="I17">
-        <v>0.281</v>
+        <v>0.243</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -13241,10 +13241,10 @@
         <v>0.003</v>
       </c>
       <c r="H18">
-        <v>0.08699999999999999</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="I18">
-        <v>0.93</v>
+        <v>0.9320000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -13270,10 +13270,10 @@
         <v>0.033</v>
       </c>
       <c r="H19">
-        <v>0.905</v>
+        <v>0.984</v>
       </c>
       <c r="I19">
-        <v>0.367</v>
+        <v>0.325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>